<commit_message>
atualização da logo das plataformas
</commit_message>
<xml_diff>
--- a/Files/indicadores_simcc/platform_image.xlsx
+++ b/Files/indicadores_simcc/platform_image.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9af2e5637b8789c0/simccv_cimatec_v4/Cubo_Iapos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{A3E611FE-DB69-40B8-8813-926900D02CAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED855CDA-CB2F-4406-8B43-788F675E7FEA}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{A3E611FE-DB69-40B8-8813-926900D02CAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9907E67-4116-4970-A733-B051536C2DC4}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{E413C054-7083-4403-A716-E0194D43DBE9}"/>
+    <workbookView xWindow="-55200" yWindow="2400" windowWidth="21600" windowHeight="11235" xr2:uid="{E413C054-7083-4403-A716-E0194D43DBE9}"/>
   </bookViews>
   <sheets>
     <sheet name="logo_platform" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">plataforma </t>
   </si>
@@ -48,9 +48,6 @@
     <t>iaPos</t>
   </si>
   <si>
-    <t>https://conectee.eng.ufmg.br/powerbi/iapos.png</t>
-  </si>
-  <si>
     <t>conectee</t>
   </si>
   <si>
@@ -67,6 +64,15 @@
   </si>
   <si>
     <t>image</t>
+  </si>
+  <si>
+    <t>npai</t>
+  </si>
+  <si>
+    <t>https://simcc.uesc.br/api/iapos.png</t>
+  </si>
+  <si>
+    <t>https://simcc.uesc.br/api/npai.png</t>
   </si>
 </sst>
 </file>
@@ -449,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6549EBCF-91E4-47DB-BE9A-F1A9A1D61E38}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -474,21 +480,30 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{10ED7F41-236D-42CD-B915-C309DABDBC4E}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{BFC74B07-EB42-41B7-B9B2-6E4A3CD28C75}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{96D222FC-AFA1-4859-916E-2A96BA78938C}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -498,7 +513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDCBC40B-EFE5-42A8-88C3-6EE1B979F298}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -510,18 +525,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>